<commit_message>
updates for physiology notes
</commit_message>
<xml_diff>
--- a/EB_041414_B.xlsx
+++ b/EB_041414_B.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="1340" windowWidth="25600" windowHeight="16060" tabRatio="624" activeTab="3"/>
+    <workbookView xWindow="3105" yWindow="1335" windowWidth="25605" windowHeight="16065" tabRatio="624" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="147">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -130,9 +135,6 @@
     <t>EMX-cre +/-</t>
   </si>
   <si>
-    <t>Injected with AAV2/9_CAGGS_flexed_ChR2_tdTomato.</t>
-  </si>
-  <si>
     <t>Burr Hole Injection</t>
   </si>
   <si>
@@ -146,6 +148,384 @@
   </si>
   <si>
     <t xml:space="preserve">Injected 100 nl of AAV2/9_CAGGS_flexed_ChR2_tdTomato. Injection site located 2.55 mm RIGHT of lambda, 350 um below pial surface. Rate of 50 nl/min. Only saw a little bit of backflow towards end of injection. </t>
+  </si>
+  <si>
+    <t>2014_05_01_0000</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Gap free, spontaneous PSCs.</t>
+  </si>
+  <si>
+    <t>2014_05_01_0001</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC steps from a FS cell, delayed onset, non-adapting. </t>
+  </si>
+  <si>
+    <t>2014_05_01_0002</t>
+  </si>
+  <si>
+    <t>2014_05_01_0003</t>
+  </si>
+  <si>
+    <t>2014_05_01_0004</t>
+  </si>
+  <si>
+    <t>2014_05_01_0005</t>
+  </si>
+  <si>
+    <t>2014_05_01_0006</t>
+  </si>
+  <si>
+    <t>2014_05_01_0007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps, 470 nm, at the soma (0 0). Very strong responses at low voltages and lots of recurrent activity. </t>
+  </si>
+  <si>
+    <t>Steps, 470 nm, at the soma (0 0). smaller step size, tons of recurrent stuff. Possibly 1.9 volts, but things are messy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps, 470 nm, at the soma (0 0). </t>
+  </si>
+  <si>
+    <t>Steps, 470 nm, at the soma (0 0). repeats, 0.8 volts. Seems better. Bit still some network stuff.</t>
+  </si>
+  <si>
+    <t>Trains, 470 nm, at ths soma, 20 Hz, not reliable PSCs on each pulse. LED set to 0.8 . FS open.</t>
+  </si>
+  <si>
+    <t>Trains, 470 nm, at ths soma, 20 Hz, 20 Hz, reliable PSCs on each pulse but lots of network activity.. LED set to 1.2 volts</t>
+  </si>
+  <si>
+    <t>2014_05_01_0008</t>
+  </si>
+  <si>
+    <t>2014_05_01_0009</t>
+  </si>
+  <si>
+    <t>2014_05_01_0010</t>
+  </si>
+  <si>
+    <t>Trains, 470 nm, at ths soma, 20 Hz, 20 Hz, reliable PSCs on each pulse but lots of network activity.. LED set to 1 volts. FS open. Less recurrent activity than with LED set to 1.2 volts. Seems like mostly depression.</t>
+  </si>
+  <si>
+    <t>2014_05_01_0011</t>
+  </si>
+  <si>
+    <t>2014_05_01_0012</t>
+  </si>
+  <si>
+    <t>2014_05_01_0013</t>
+  </si>
+  <si>
+    <t>2014_05_01_0014</t>
+  </si>
+  <si>
+    <t>Steps, 470 nm, at (-315 156). FS closed. 2 volts seem good</t>
+  </si>
+  <si>
+    <t>Steps, 470 nm, at (-315 156). FS closed. Repeats of 2 volts.</t>
+  </si>
+  <si>
+    <t>Trains, 20 Hz, 470 nm, at (-315 156). FS closed. LED set to 2 Volts. Seems like mostly depression.</t>
+  </si>
+  <si>
+    <t>Trains, 40 Hz, 470 nm, at (-315 156). FS closed. LED set to 2 Volts. Seems like mostly depression. Series resistance is getting worse.</t>
+  </si>
+  <si>
+    <t>2014_05_01_0015</t>
+  </si>
+  <si>
+    <t>2014_05_01_0016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trains, 5 Hz, 470 nm, at (-315 156). FS closed. LED set to 2 Volts. </t>
+  </si>
+  <si>
+    <t>2014_05_01_0017</t>
+  </si>
+  <si>
+    <t>2014_05_01_0018</t>
+  </si>
+  <si>
+    <t>2014_05_01_0019</t>
+  </si>
+  <si>
+    <t>2014_05_01_0020</t>
+  </si>
+  <si>
+    <t>2014_05_01_0021</t>
+  </si>
+  <si>
+    <t>Steps, 5 volts, repeats at (-299 184)). Using the tdTomato cube. Strong responses, maybe just above L5. Looking to see if the activity is restricted to a certain band. FS closed</t>
+  </si>
+  <si>
+    <t>Steps, 5 volts, repeats at (-341 227). Using the tdTomato cube. Strong responses, probably at L5. Looking to see if the activity is restricted to a certain band. FS closed</t>
+  </si>
+  <si>
+    <t>Steps, 5 volts, repeats at (-360 241). Using the tdTomato cube. Measurable responses, presumbably below L5. Looking to see if the activity is restricted to a certain band. FS closed</t>
+  </si>
+  <si>
+    <t>Steps, 5 volts, repeats at (-417 278). Using the tdTomato cube. Small responses, presumbably below L5). Looking to see if the activity is restricted to a certain band. FS closed</t>
+  </si>
+  <si>
+    <t>Trains 20 Hz, 470 nm, at (-341, 227), FS closed. Using the mCherry cube again. Acess getting worse again.</t>
+  </si>
+  <si>
+    <t>Wash in 10 uM NBQX and APV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps, 10 volts, at (-341 227), FS closed. In synaptic blockers. </t>
+  </si>
+  <si>
+    <t>Steps, 10 volts, at the soma (0 0), FS open. In synaptic blockers. About a 10 pA response.</t>
+  </si>
+  <si>
+    <t>2014_05_01_0022</t>
+  </si>
+  <si>
+    <t>In current clamp. Steps, 10 volts, at the soma (0 0), FS open. In synaptic blockers. About a 2 mV response.</t>
+  </si>
+  <si>
+    <t>DC steps to confrim cell health. Things have definitely deteriorated, but it still produces dinky little spikes….</t>
+  </si>
+  <si>
+    <t>out</t>
+  </si>
+  <si>
+    <t>Pia at about (236 -113). Vout = 7 mV.</t>
+  </si>
+  <si>
+    <t>DC steps from a  layer 5 PY cell.</t>
+  </si>
+  <si>
+    <t>2014_05_01_0023</t>
+  </si>
+  <si>
+    <t>LED steps, FS open at the soma. Weak responses, but this is after synaptic blockers had been used on this slice (in normal acsf for this file).</t>
+  </si>
+  <si>
+    <t>LED steps at (177 -136). Presumably at the L2/3 apical dendrite location. (during washin of blockers…). FS open.</t>
+  </si>
+  <si>
+    <t>in the presense of blockers. 10 volts to LED. At ths apical dendrite location. FS open. Very weak response.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">still in blockers, at the soma (0 0). FS open. Very small response. 10 volt repeats. </t>
+  </si>
+  <si>
+    <t>With -10pA holding current, 10 volt pulses from the LED. In current clamp, about 1 mV of depolarization, Light at the soma. FS open.</t>
+  </si>
+  <si>
+    <t>2014_05_01_0024</t>
+  </si>
+  <si>
+    <t>2014_05_01_0025</t>
+  </si>
+  <si>
+    <t>2014_05_01_0026</t>
+  </si>
+  <si>
+    <t>2014_05_01_0027</t>
+  </si>
+  <si>
+    <t>2014_05_01_0028</t>
+  </si>
+  <si>
+    <t>2014_05_01_0029</t>
+  </si>
+  <si>
+    <t>DC steps to confirm cell health. Still good. Usint -10 pA holding current.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pia at (500 -330), Vout = 1 mV. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Callosum is not yet fused. Strong signal in the thalamus, weak signal in the SC. Hippocampus is migrating dorsally, but not yet consolidated. At least 2 HVAs present. One is lateral of V1 and the other(s) are medial. The medial complex is wedge shaped and my be a single area or two areas that are fused in this slice (PM + AM?). </t>
+  </si>
+  <si>
+    <t>2014_05_01_0030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gap free, spontaneous PSCs. </t>
+  </si>
+  <si>
+    <t>2014_05_01_0031</t>
+  </si>
+  <si>
+    <t>2014_05_01_0032</t>
+  </si>
+  <si>
+    <t>2014_05_01_0033</t>
+  </si>
+  <si>
+    <t>2014_05_01_0034</t>
+  </si>
+  <si>
+    <t>2014_05_01_0035</t>
+  </si>
+  <si>
+    <t>2014_05_01_0036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steps, at the soma (0 0). 470 nm, FS open.  2.5 or 3 Volts yield good responses. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trains, 20 Hz, at the soma (0 0). FS open. LED set to 3 volts. </t>
+  </si>
+  <si>
+    <t>Steps, 470 nm, at (-198 187), FS closed. 10 volts was good, 8 was ok too.</t>
+  </si>
+  <si>
+    <t>Trains 20 Hz, 470 nm, at (-198 187), FS closed. 8 volts. Seems like depression, but at the soma it seemed like there was PPfacil.</t>
+  </si>
+  <si>
+    <t>Trains 40 Hz, 470 nm, at (-198 187), FS closed. 8 volts. A few sweeps have some spontaneous PSCs and should potentially be deleted.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trains 40 Hz, 470 nm, at (-198 187), FS closed. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>10 volts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>. Seems like roughly the same thing as with 8 volts, although possibly more profound depression (false depression?)</t>
+    </r>
+  </si>
+  <si>
+    <t>2014_05_01_0037</t>
+  </si>
+  <si>
+    <t>2014_05_01_0038</t>
+  </si>
+  <si>
+    <t>2014_05_01_0039</t>
+  </si>
+  <si>
+    <t>2014_05_01_0040</t>
+  </si>
+  <si>
+    <t>Trains 5 Hz, 470 nm, at (-198 187), FS closed. 8 volts. Access got a little worse.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trains 5 Hz, 470 nm, at (-198 187), FS closed. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>10 volts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>K-Gluconate ('Busted')</t>
+  </si>
+  <si>
+    <t>Normal, some files have 10 uM NBQX and APV.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trains 20 Hz, 470 nm, at (-198 187), FS closed. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>10 volts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">. A few sweeps for comparison with the file when the LED was set to 8 volts. </t>
+    </r>
+  </si>
+  <si>
+    <t>2014_05_01_0041</t>
+  </si>
+  <si>
+    <t>2014_05_01_0042</t>
+  </si>
+  <si>
+    <t>2014_05_01_0043</t>
+  </si>
+  <si>
+    <t>2014_05_01_0044</t>
+  </si>
+  <si>
+    <t>Trains 20 Hz, 470 nm, at (-307 187), FS closed. 10 volts. Seems like small PPfacil (consistent with soma, but not the 1st distal stim location).</t>
+  </si>
+  <si>
+    <t>Trains 40 Hz, 470 nm, at (-307 187), FS closed. 10 volts. Looks like depression is more dominant, but a few sweeps have facilitation.</t>
+  </si>
+  <si>
+    <t>Trains 5 Hz, 470 nm, at (-307 187), FS closed. 10 volts. Funky stuff on one sweep. Might need to eliminate this sweep.</t>
+  </si>
+  <si>
+    <t>2014_05_01_0045</t>
+  </si>
+  <si>
+    <t>Good signal in the deep layers of the SC. No signal in the thalamus, I think that the MGN is present but not the LGN. There are 2 HVAs present. Possibly AL and PM. PM is weaker expression, and the lateral complex may be a combination of LM and AL</t>
+  </si>
+  <si>
+    <t>DC steps from a L2/3 PY cell. Possibly in PM.</t>
+  </si>
+  <si>
+    <t>In synaptic blockers. 10 uM APV and NBQX. LED 470 nm steps at soma with the FS iris open.</t>
+  </si>
+  <si>
+    <t>In synaptic blockers. 10 uM APV and NBQX. LED 470 nm steps at soma with the FS iris open. In current clamp.</t>
+  </si>
+  <si>
+    <t>DC steps to demonstrate cell health is still ok after blockers were washed on.</t>
+  </si>
+  <si>
+    <t>Pia at (148 -109). Vout = 3 mV.</t>
+  </si>
+  <si>
+    <t>Recording from HVAs looking at freq dependence of STP. One FS cell from PM(?). One L5 cell from PM(?) demonstrating lack of retrograde expression. Another L2/3 PY cell from PM(?)</t>
+  </si>
+  <si>
+    <t>Injected with AAV2/9_CAGGS_flexed_ChR2_tdTomato. Whole cell recording from HVAs looking at TF dependence of STP. Histology.</t>
+  </si>
+  <si>
+    <t>4% pfa</t>
   </si>
 </sst>
 </file>
@@ -155,7 +535,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -685,7 +1065,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -787,6 +1167,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -795,15 +1187,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -894,6 +1277,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -905,21 +1303,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1271,25 +1654,25 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="38" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="38.1" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="20.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="62.375" style="27" customWidth="1"/>
     <col min="3" max="16384" width="18.5" style="9" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="38" customHeight="1" thickTop="1">
+    <row r="1" spans="1:2" ht="38.1" customHeight="1" thickTop="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="38" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="38.1" customHeight="1">
       <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
@@ -1297,7 +1680,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="38" customHeight="1">
+    <row r="3" spans="1:2" ht="38.1" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1305,7 +1688,7 @@
         <v>41714</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="38" customHeight="1">
+    <row r="4" spans="1:2" ht="38.1" customHeight="1">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1313,35 +1696,35 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="38" customHeight="1">
+    <row r="5" spans="1:2" ht="38.1" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="148" customHeight="1" thickBot="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="147.94999999999999" customHeight="1" thickBot="1">
       <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="38" hidden="1" customHeight="1" thickTop="1"/>
-    <row r="8" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="9" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="10" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="11" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="12" spans="1:2" ht="38" hidden="1" customHeight="1"/>
-    <row r="13" spans="1:2" ht="38" hidden="1" customHeight="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="38.1" hidden="1" customHeight="1" thickTop="1"/>
+    <row r="8" spans="1:2" ht="38.1" hidden="1" customHeight="1"/>
+    <row r="9" spans="1:2" ht="38.1" hidden="1" customHeight="1"/>
+    <row r="10" spans="1:2" ht="38.1" hidden="1" customHeight="1"/>
+    <row r="11" spans="1:2" ht="38.1" hidden="1" customHeight="1"/>
+    <row r="12" spans="1:2" ht="38.1" hidden="1" customHeight="1"/>
+    <row r="13" spans="1:2" ht="38.1" hidden="1" customHeight="1">
       <c r="A13" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>
@@ -1354,84 +1737,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="6.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" style="21" customWidth="1"/>
     <col min="6" max="6" width="34.5" style="21" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="15" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" thickTop="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="22">
+        <v>297</v>
+      </c>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="24">
+        <v>305</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="39" customHeight="1">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="42">
+        <v>34</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
     </row>
     <row r="4" spans="1:8" ht="102" customHeight="1" thickBot="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47"/>
-    </row>
-    <row r="5" spans="1:8" ht="26" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
+    </row>
+    <row r="5" spans="1:8" ht="26.1" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" thickTop="1">
       <c r="A6" s="6" t="s">
@@ -1449,271 +1844,565 @@
       <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="39"/>
-    </row>
-    <row r="7" spans="1:8" ht="39" customHeight="1">
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:8" ht="98.25" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5">
+        <v>6</v>
+      </c>
       <c r="E7" s="23"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36"/>
+      <c r="F7" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="39"/>
+      <c r="H7" s="40"/>
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="5">
+        <v>6</v>
+      </c>
+      <c r="E8" s="23">
+        <v>-72</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" ht="39" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
-    </row>
-    <row r="10" spans="1:8" ht="39" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="34">
+        <v>6</v>
+      </c>
+      <c r="E9" s="23">
+        <v>-70</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+    </row>
+    <row r="10" spans="1:8" ht="52.5" customHeight="1">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="34">
+        <v>6</v>
+      </c>
+      <c r="E10" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="34">
+        <v>6</v>
+      </c>
+      <c r="E11" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:8" ht="39" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="36"/>
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="34">
+        <v>6</v>
+      </c>
+      <c r="E12" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="39"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:8" ht="39" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="34">
+        <v>6</v>
+      </c>
+      <c r="E13" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:8" ht="39" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
-    </row>
-    <row r="15" spans="1:8" ht="39" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
-    </row>
-    <row r="16" spans="1:8" ht="39" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
-    </row>
-    <row r="17" spans="1:8" ht="39" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="34">
+        <v>6</v>
+      </c>
+      <c r="E14" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
+    </row>
+    <row r="15" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="34">
+        <v>6</v>
+      </c>
+      <c r="E15" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="39"/>
+      <c r="H15" s="40"/>
+    </row>
+    <row r="16" spans="1:8" ht="84" customHeight="1">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="34">
+        <v>6</v>
+      </c>
+      <c r="E16" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="39"/>
+      <c r="H16" s="40"/>
+    </row>
+    <row r="17" spans="1:8" ht="48.75" customHeight="1">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="34">
+        <v>6</v>
+      </c>
+      <c r="E17" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40"/>
     </row>
     <row r="18" spans="1:8" ht="39" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
-    </row>
-    <row r="19" spans="1:8" ht="39" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="36"/>
-    </row>
-    <row r="20" spans="1:8" ht="39" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
-    </row>
-    <row r="21" spans="1:8" ht="39" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="36"/>
-    </row>
-    <row r="22" spans="1:8" ht="39" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
-    </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36"/>
-    </row>
-    <row r="24" spans="1:8" ht="39" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="36"/>
-    </row>
-    <row r="25" spans="1:8" ht="39" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="36"/>
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="34">
+        <v>6</v>
+      </c>
+      <c r="E18" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="39"/>
+      <c r="H18" s="40"/>
+    </row>
+    <row r="19" spans="1:8" ht="50.25" customHeight="1">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="34">
+        <v>6</v>
+      </c>
+      <c r="E19" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="39"/>
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20" spans="1:8" ht="59.25" customHeight="1">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="34">
+        <v>6</v>
+      </c>
+      <c r="E20" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="39"/>
+      <c r="H20" s="40"/>
+    </row>
+    <row r="21" spans="1:8" ht="72" customHeight="1">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="34">
+        <v>6</v>
+      </c>
+      <c r="E21" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="39"/>
+      <c r="H21" s="40"/>
+    </row>
+    <row r="22" spans="1:8" ht="67.5" customHeight="1">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="34">
+        <v>6</v>
+      </c>
+      <c r="E22" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="39"/>
+      <c r="H22" s="40"/>
+    </row>
+    <row r="23" spans="1:8" ht="71.25" customHeight="1">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="34">
+        <v>6</v>
+      </c>
+      <c r="E23" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="39"/>
+      <c r="H23" s="40"/>
+    </row>
+    <row r="24" spans="1:8" ht="61.5" customHeight="1">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="34">
+        <v>6</v>
+      </c>
+      <c r="E24" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
+    </row>
+    <row r="25" spans="1:8" ht="55.5" customHeight="1">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="34">
+        <v>6</v>
+      </c>
+      <c r="E25" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="39"/>
+      <c r="H25" s="40"/>
     </row>
     <row r="26" spans="1:8" ht="39" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="34">
+        <v>6</v>
+      </c>
+      <c r="E26" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="39"/>
+      <c r="H26" s="40"/>
     </row>
     <row r="27" spans="1:8" ht="39" customHeight="1">
-      <c r="A27" s="3"/>
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="36"/>
+      <c r="D27" s="34">
+        <v>6</v>
+      </c>
+      <c r="E27" s="34"/>
+      <c r="F27" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="39"/>
+      <c r="H27" s="40"/>
     </row>
     <row r="28" spans="1:8" ht="39" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="36"/>
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="34">
+        <v>6</v>
+      </c>
+      <c r="E28" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F28" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="39"/>
+      <c r="H28" s="40"/>
     </row>
     <row r="29" spans="1:8" ht="39" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="34">
+        <v>6</v>
+      </c>
+      <c r="E29" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F29" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="39"/>
+      <c r="H29" s="40"/>
     </row>
     <row r="30" spans="1:8" ht="39" customHeight="1">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="36"/>
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="34">
+        <v>6</v>
+      </c>
+      <c r="E30" s="34">
+        <v>-66</v>
+      </c>
+      <c r="F30" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
     </row>
     <row r="31" spans="1:8" ht="39" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="36"/>
+      <c r="A31" s="3">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="34">
+        <v>6</v>
+      </c>
+      <c r="E31" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F31" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
     </row>
     <row r="32" spans="1:8" ht="39" customHeight="1">
-      <c r="A32" s="3"/>
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
+      <c r="D32" s="34">
+        <v>6</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="39"/>
+      <c r="H32" s="40"/>
     </row>
     <row r="33" spans="1:8" ht="39" customHeight="1">
       <c r="A33" s="3"/>
@@ -1721,89 +2410,181 @@
       <c r="C33" s="4"/>
       <c r="D33" s="5"/>
       <c r="E33" s="23"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="36"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="40"/>
     </row>
     <row r="34" spans="1:8" ht="39" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="36"/>
-    </row>
-    <row r="35" spans="1:8" ht="39" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="36"/>
+      <c r="A34" s="3">
+        <v>2</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="5">
+        <v>6</v>
+      </c>
+      <c r="E34" s="23">
+        <v>-68</v>
+      </c>
+      <c r="F34" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="39"/>
+      <c r="H34" s="40"/>
+    </row>
+    <row r="35" spans="1:8" ht="60" customHeight="1">
+      <c r="A35" s="3">
+        <v>2</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="34">
+        <v>6</v>
+      </c>
+      <c r="E35" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F35" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="39"/>
+      <c r="H35" s="40"/>
     </row>
     <row r="36" spans="1:8" ht="39" customHeight="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="36"/>
+      <c r="A36" s="3">
+        <v>2</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="34">
+        <v>6</v>
+      </c>
+      <c r="E36" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F36" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="39"/>
+      <c r="H36" s="40"/>
     </row>
     <row r="37" spans="1:8" ht="39" customHeight="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="36"/>
+      <c r="A37" s="3">
+        <v>2</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="34">
+        <v>6</v>
+      </c>
+      <c r="E37" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F37" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="39"/>
+      <c r="H37" s="40"/>
     </row>
     <row r="38" spans="1:8" ht="39" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="36"/>
-    </row>
-    <row r="39" spans="1:8" ht="39" customHeight="1">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="36"/>
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="34">
+        <v>6</v>
+      </c>
+      <c r="E38" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="40"/>
+    </row>
+    <row r="39" spans="1:8" ht="53.25" customHeight="1">
+      <c r="A39" s="3">
+        <v>2</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="34">
+        <v>6</v>
+      </c>
+      <c r="E39" s="23">
+        <v>-65</v>
+      </c>
+      <c r="F39" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="G39" s="39"/>
+      <c r="H39" s="40"/>
     </row>
     <row r="40" spans="1:8" ht="39" customHeight="1">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="36"/>
+      <c r="A40" s="3">
+        <v>2</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="34">
+        <v>6</v>
+      </c>
+      <c r="E40" s="23">
+        <v>-68</v>
+      </c>
+      <c r="F40" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="39"/>
+      <c r="H40" s="40"/>
     </row>
     <row r="41" spans="1:8" ht="39" customHeight="1">
-      <c r="A41" s="3"/>
+      <c r="A41" s="3">
+        <v>2</v>
+      </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="36"/>
+      <c r="D41" s="34">
+        <v>6</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="G41" s="39"/>
+      <c r="H41" s="40"/>
     </row>
     <row r="42" spans="1:8" ht="39" customHeight="1">
       <c r="A42" s="3"/>
@@ -1811,199 +2592,405 @@
       <c r="C42" s="4"/>
       <c r="D42" s="5"/>
       <c r="E42" s="23"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="36"/>
-    </row>
-    <row r="43" spans="1:8" ht="39" customHeight="1">
+      <c r="F42" s="38"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="40"/>
+    </row>
+    <row r="43" spans="1:8" ht="83.25" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5">
+        <v>5</v>
+      </c>
       <c r="E43" s="23"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="36"/>
+      <c r="F43" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43" s="39"/>
+      <c r="H43" s="40"/>
     </row>
     <row r="44" spans="1:8" ht="39" customHeight="1">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="36"/>
+      <c r="A44" s="3">
+        <v>3</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="5">
+        <v>5</v>
+      </c>
+      <c r="E44" s="23">
+        <v>-75</v>
+      </c>
+      <c r="F44" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="39"/>
+      <c r="H44" s="40"/>
     </row>
     <row r="45" spans="1:8" ht="39" customHeight="1">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="36"/>
+      <c r="A45" s="3">
+        <v>3</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="34">
+        <v>5</v>
+      </c>
+      <c r="E45" s="23">
+        <v>-76</v>
+      </c>
+      <c r="F45" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="G45" s="39"/>
+      <c r="H45" s="40"/>
     </row>
     <row r="46" spans="1:8" ht="39" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="36"/>
+      <c r="A46" s="3">
+        <v>3</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="34">
+        <v>5</v>
+      </c>
+      <c r="E46" s="23">
+        <v>-85</v>
+      </c>
+      <c r="F46" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="G46" s="39"/>
+      <c r="H46" s="40"/>
     </row>
     <row r="47" spans="1:8" ht="39" customHeight="1">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="36"/>
+      <c r="A47" s="3">
+        <v>3</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="34">
+        <v>5</v>
+      </c>
+      <c r="E47" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F47" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="G47" s="39"/>
+      <c r="H47" s="40"/>
     </row>
     <row r="48" spans="1:8" ht="39" customHeight="1">
-      <c r="A48" s="3"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="36"/>
-    </row>
-    <row r="49" spans="1:8" ht="39" customHeight="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="36"/>
-    </row>
-    <row r="50" spans="1:8" ht="39" customHeight="1">
-      <c r="A50" s="3"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="36"/>
-    </row>
-    <row r="51" spans="1:8" ht="39" customHeight="1">
-      <c r="A51" s="3"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="36"/>
-    </row>
-    <row r="52" spans="1:8" ht="39" customHeight="1">
-      <c r="A52" s="3"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="36"/>
-    </row>
-    <row r="53" spans="1:8" ht="39" customHeight="1">
-      <c r="A53" s="3"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="36"/>
-    </row>
-    <row r="54" spans="1:8" ht="39" customHeight="1">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="36"/>
-    </row>
-    <row r="55" spans="1:8" ht="39" customHeight="1">
-      <c r="A55" s="3"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="36"/>
-    </row>
-    <row r="56" spans="1:8" ht="39" customHeight="1">
-      <c r="A56" s="3"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="36"/>
-    </row>
-    <row r="57" spans="1:8" ht="39" customHeight="1">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="36"/>
-    </row>
-    <row r="58" spans="1:8" ht="39" customHeight="1">
-      <c r="A58" s="3"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="36"/>
+      <c r="A48" s="3">
+        <v>3</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="34">
+        <v>5</v>
+      </c>
+      <c r="E48" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F48" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" s="39"/>
+      <c r="H48" s="40"/>
+    </row>
+    <row r="49" spans="1:8" ht="59.25" customHeight="1">
+      <c r="A49" s="3">
+        <v>3</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="34">
+        <v>5</v>
+      </c>
+      <c r="E49" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="G49" s="39"/>
+      <c r="H49" s="40"/>
+    </row>
+    <row r="50" spans="1:8" ht="77.25" customHeight="1">
+      <c r="A50" s="3">
+        <v>3</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="34">
+        <v>5</v>
+      </c>
+      <c r="E50" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F50" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="G50" s="39"/>
+      <c r="H50" s="40"/>
+    </row>
+    <row r="51" spans="1:8" ht="74.25" customHeight="1">
+      <c r="A51" s="3">
+        <v>3</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="34">
+        <v>5</v>
+      </c>
+      <c r="E51" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F51" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="G51" s="39"/>
+      <c r="H51" s="40"/>
+    </row>
+    <row r="52" spans="1:8" ht="62.25" customHeight="1">
+      <c r="A52" s="3">
+        <v>3</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="34">
+        <v>5</v>
+      </c>
+      <c r="E52" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F52" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" s="39"/>
+      <c r="H52" s="40"/>
+    </row>
+    <row r="53" spans="1:8" ht="45" customHeight="1">
+      <c r="A53" s="3">
+        <v>3</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" s="34">
+        <v>5</v>
+      </c>
+      <c r="E53" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F53" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" s="39"/>
+      <c r="H53" s="40"/>
+    </row>
+    <row r="54" spans="1:8" ht="60.75" customHeight="1">
+      <c r="A54" s="3">
+        <v>3</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="34">
+        <v>5</v>
+      </c>
+      <c r="E54" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F54" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="G54" s="39"/>
+      <c r="H54" s="40"/>
+    </row>
+    <row r="55" spans="1:8" ht="73.5" customHeight="1">
+      <c r="A55" s="3">
+        <v>3</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" s="34">
+        <v>5</v>
+      </c>
+      <c r="E55" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F55" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G55" s="39"/>
+      <c r="H55" s="40"/>
+    </row>
+    <row r="56" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A56" s="3">
+        <v>3</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="34">
+        <v>5</v>
+      </c>
+      <c r="E56" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F56" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="G56" s="39"/>
+      <c r="H56" s="40"/>
+    </row>
+    <row r="57" spans="1:8" ht="56.25" customHeight="1">
+      <c r="A57" s="3">
+        <v>3</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D57" s="34">
+        <v>5</v>
+      </c>
+      <c r="E57" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F57" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="G57" s="39"/>
+      <c r="H57" s="40"/>
+    </row>
+    <row r="58" spans="1:8" ht="52.5" customHeight="1">
+      <c r="A58" s="3">
+        <v>3</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="34">
+        <v>5</v>
+      </c>
+      <c r="E58" s="34">
+        <v>-85</v>
+      </c>
+      <c r="F58" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="G58" s="39"/>
+      <c r="H58" s="40"/>
     </row>
     <row r="59" spans="1:8" ht="39" customHeight="1">
-      <c r="A59" s="3"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="5"/>
+      <c r="A59" s="3">
+        <v>3</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D59" s="34">
+        <v>5</v>
+      </c>
       <c r="E59" s="23"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="36"/>
+      <c r="F59" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="39"/>
+      <c r="H59" s="40"/>
     </row>
     <row r="60" spans="1:8" ht="39" customHeight="1">
-      <c r="A60" s="3"/>
+      <c r="A60" s="3">
+        <v>3</v>
+      </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
-      <c r="D60" s="5"/>
+      <c r="D60" s="34">
+        <v>5</v>
+      </c>
       <c r="E60" s="23"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="36"/>
+      <c r="F60" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G60" s="39"/>
+      <c r="H60" s="40"/>
     </row>
     <row r="61" spans="1:8" ht="39" customHeight="1">
-      <c r="A61" s="3"/>
+      <c r="A61" s="3">
+        <v>3</v>
+      </c>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="34">
+        <v>5</v>
+      </c>
       <c r="E61" s="23"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="36"/>
+      <c r="F61" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="G61" s="39"/>
+      <c r="H61" s="40"/>
     </row>
     <row r="62" spans="1:8" ht="39" customHeight="1">
       <c r="A62" s="3"/>
@@ -2011,9 +2998,9 @@
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
       <c r="E62" s="23"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="36"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="40"/>
     </row>
     <row r="63" spans="1:8" ht="39" customHeight="1">
       <c r="A63" s="3"/>
@@ -2021,9 +3008,9 @@
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="23"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="36"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="40"/>
     </row>
     <row r="64" spans="1:8" ht="39" customHeight="1">
       <c r="A64" s="3"/>
@@ -2031,9 +3018,9 @@
       <c r="C64" s="4"/>
       <c r="D64" s="5"/>
       <c r="E64" s="23"/>
-      <c r="F64" s="34"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="36"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="40"/>
     </row>
     <row r="65" spans="1:8" ht="39" customHeight="1">
       <c r="A65" s="3"/>
@@ -2041,9 +3028,9 @@
       <c r="C65" s="4"/>
       <c r="D65" s="5"/>
       <c r="E65" s="23"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="36"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="40"/>
     </row>
     <row r="66" spans="1:8" ht="39" customHeight="1">
       <c r="A66" s="3"/>
@@ -2051,9 +3038,9 @@
       <c r="C66" s="4"/>
       <c r="D66" s="5"/>
       <c r="E66" s="23"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="36"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="40"/>
     </row>
     <row r="67" spans="1:8" ht="39" customHeight="1">
       <c r="A67" s="3"/>
@@ -2061,9 +3048,9 @@
       <c r="C67" s="4"/>
       <c r="D67" s="5"/>
       <c r="E67" s="23"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="36"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="40"/>
     </row>
     <row r="68" spans="1:8" ht="39" customHeight="1">
       <c r="A68" s="3"/>
@@ -2071,9 +3058,9 @@
       <c r="C68" s="4"/>
       <c r="D68" s="5"/>
       <c r="E68" s="23"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="36"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="40"/>
     </row>
     <row r="69" spans="1:8" ht="39" customHeight="1">
       <c r="A69" s="3"/>
@@ -2081,9 +3068,9 @@
       <c r="C69" s="4"/>
       <c r="D69" s="5"/>
       <c r="E69" s="23"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="35"/>
-      <c r="H69" s="36"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="40"/>
     </row>
     <row r="70" spans="1:8" ht="39" customHeight="1">
       <c r="A70" s="3"/>
@@ -2091,9 +3078,9 @@
       <c r="C70" s="4"/>
       <c r="D70" s="5"/>
       <c r="E70" s="23"/>
-      <c r="F70" s="34"/>
-      <c r="G70" s="35"/>
-      <c r="H70" s="36"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="40"/>
     </row>
     <row r="71" spans="1:8" ht="39" customHeight="1">
       <c r="A71" s="3"/>
@@ -2101,9 +3088,9 @@
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="23"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="36"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="40"/>
     </row>
     <row r="72" spans="1:8" ht="39" customHeight="1">
       <c r="A72" s="3"/>
@@ -2111,9 +3098,9 @@
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
       <c r="E72" s="23"/>
-      <c r="F72" s="34"/>
-      <c r="G72" s="35"/>
-      <c r="H72" s="36"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="40"/>
     </row>
     <row r="73" spans="1:8" ht="39" customHeight="1">
       <c r="A73" s="3"/>
@@ -2121,9 +3108,9 @@
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="23"/>
-      <c r="F73" s="34"/>
-      <c r="G73" s="35"/>
-      <c r="H73" s="36"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="39"/>
+      <c r="H73" s="40"/>
     </row>
     <row r="74" spans="1:8" ht="39" customHeight="1">
       <c r="A74" s="3"/>
@@ -2131,9 +3118,9 @@
       <c r="C74" s="4"/>
       <c r="D74" s="5"/>
       <c r="E74" s="23"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="35"/>
-      <c r="H74" s="36"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
+      <c r="H74" s="40"/>
     </row>
     <row r="75" spans="1:8" ht="39" customHeight="1">
       <c r="A75" s="3"/>
@@ -2141,9 +3128,9 @@
       <c r="C75" s="4"/>
       <c r="D75" s="5"/>
       <c r="E75" s="23"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="36"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="40"/>
     </row>
     <row r="76" spans="1:8" ht="39" customHeight="1">
       <c r="A76" s="3"/>
@@ -2151,9 +3138,9 @@
       <c r="C76" s="4"/>
       <c r="D76" s="5"/>
       <c r="E76" s="23"/>
-      <c r="F76" s="34"/>
-      <c r="G76" s="35"/>
-      <c r="H76" s="36"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="39"/>
+      <c r="H76" s="40"/>
     </row>
     <row r="77" spans="1:8" ht="39" customHeight="1">
       <c r="A77" s="3"/>
@@ -2161,9 +3148,9 @@
       <c r="C77" s="4"/>
       <c r="D77" s="5"/>
       <c r="E77" s="23"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="35"/>
-      <c r="H77" s="36"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="39"/>
+      <c r="H77" s="40"/>
     </row>
     <row r="78" spans="1:8" ht="39" customHeight="1">
       <c r="A78" s="3"/>
@@ -2171,9 +3158,9 @@
       <c r="C78" s="4"/>
       <c r="D78" s="5"/>
       <c r="E78" s="23"/>
-      <c r="F78" s="34"/>
-      <c r="G78" s="35"/>
-      <c r="H78" s="36"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="39"/>
+      <c r="H78" s="40"/>
     </row>
     <row r="79" spans="1:8" ht="39" customHeight="1">
       <c r="A79" s="3"/>
@@ -2181,9 +3168,9 @@
       <c r="C79" s="4"/>
       <c r="D79" s="5"/>
       <c r="E79" s="23"/>
-      <c r="F79" s="34"/>
-      <c r="G79" s="35"/>
-      <c r="H79" s="36"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="40"/>
     </row>
     <row r="80" spans="1:8" ht="39" customHeight="1">
       <c r="A80" s="3"/>
@@ -2191,9 +3178,9 @@
       <c r="C80" s="4"/>
       <c r="D80" s="5"/>
       <c r="E80" s="23"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="35"/>
-      <c r="H80" s="36"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="40"/>
     </row>
     <row r="81" spans="1:8" ht="39" customHeight="1">
       <c r="A81" s="3"/>
@@ -2201,9 +3188,9 @@
       <c r="C81" s="4"/>
       <c r="D81" s="5"/>
       <c r="E81" s="23"/>
-      <c r="F81" s="34"/>
-      <c r="G81" s="35"/>
-      <c r="H81" s="36"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="39"/>
+      <c r="H81" s="40"/>
     </row>
     <row r="82" spans="1:8" ht="39" customHeight="1">
       <c r="A82" s="3"/>
@@ -2211,9 +3198,9 @@
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="23"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="35"/>
-      <c r="H82" s="36"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="39"/>
+      <c r="H82" s="40"/>
     </row>
     <row r="83" spans="1:8" ht="39" customHeight="1">
       <c r="A83" s="3"/>
@@ -2221,9 +3208,9 @@
       <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="23"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="35"/>
-      <c r="H83" s="36"/>
+      <c r="F83" s="38"/>
+      <c r="G83" s="39"/>
+      <c r="H83" s="40"/>
     </row>
     <row r="84" spans="1:8" ht="39" customHeight="1">
       <c r="A84" s="3"/>
@@ -2231,9 +3218,9 @@
       <c r="C84" s="4"/>
       <c r="D84" s="5"/>
       <c r="E84" s="23"/>
-      <c r="F84" s="34"/>
-      <c r="G84" s="35"/>
-      <c r="H84" s="36"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="39"/>
+      <c r="H84" s="40"/>
     </row>
     <row r="85" spans="1:8" ht="39" customHeight="1">
       <c r="A85" s="3"/>
@@ -2241,9 +3228,9 @@
       <c r="C85" s="4"/>
       <c r="D85" s="5"/>
       <c r="E85" s="23"/>
-      <c r="F85" s="34"/>
-      <c r="G85" s="35"/>
-      <c r="H85" s="36"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="39"/>
+      <c r="H85" s="40"/>
     </row>
     <row r="86" spans="1:8" ht="39" customHeight="1">
       <c r="A86" s="3"/>
@@ -2251,9 +3238,9 @@
       <c r="C86" s="4"/>
       <c r="D86" s="5"/>
       <c r="E86" s="23"/>
-      <c r="F86" s="34"/>
-      <c r="G86" s="35"/>
-      <c r="H86" s="36"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="40"/>
     </row>
     <row r="87" spans="1:8" ht="39" customHeight="1">
       <c r="A87" s="3"/>
@@ -2261,9 +3248,9 @@
       <c r="C87" s="4"/>
       <c r="D87" s="5"/>
       <c r="E87" s="23"/>
-      <c r="F87" s="34"/>
-      <c r="G87" s="35"/>
-      <c r="H87" s="36"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="39"/>
+      <c r="H87" s="40"/>
     </row>
     <row r="88" spans="1:8" ht="39" customHeight="1">
       <c r="A88" s="3"/>
@@ -2271,9 +3258,9 @@
       <c r="C88" s="4"/>
       <c r="D88" s="5"/>
       <c r="E88" s="23"/>
-      <c r="F88" s="34"/>
-      <c r="G88" s="35"/>
-      <c r="H88" s="36"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="39"/>
+      <c r="H88" s="40"/>
     </row>
     <row r="89" spans="1:8" ht="39" customHeight="1">
       <c r="A89" s="3"/>
@@ -2281,9 +3268,9 @@
       <c r="C89" s="4"/>
       <c r="D89" s="5"/>
       <c r="E89" s="23"/>
-      <c r="F89" s="34"/>
-      <c r="G89" s="35"/>
-      <c r="H89" s="36"/>
+      <c r="F89" s="38"/>
+      <c r="G89" s="39"/>
+      <c r="H89" s="40"/>
     </row>
     <row r="90" spans="1:8" ht="39" customHeight="1">
       <c r="A90" s="3"/>
@@ -2291,9 +3278,9 @@
       <c r="C90" s="4"/>
       <c r="D90" s="5"/>
       <c r="E90" s="23"/>
-      <c r="F90" s="34"/>
-      <c r="G90" s="35"/>
-      <c r="H90" s="36"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="39"/>
+      <c r="H90" s="40"/>
     </row>
     <row r="91" spans="1:8" ht="39" customHeight="1">
       <c r="A91" s="3"/>
@@ -2301,9 +3288,9 @@
       <c r="C91" s="4"/>
       <c r="D91" s="5"/>
       <c r="E91" s="23"/>
-      <c r="F91" s="34"/>
-      <c r="G91" s="35"/>
-      <c r="H91" s="36"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="40"/>
     </row>
     <row r="92" spans="1:8" ht="39" customHeight="1">
       <c r="A92" s="3"/>
@@ -2311,9 +3298,9 @@
       <c r="C92" s="4"/>
       <c r="D92" s="5"/>
       <c r="E92" s="23"/>
-      <c r="F92" s="34"/>
-      <c r="G92" s="35"/>
-      <c r="H92" s="36"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="39"/>
+      <c r="H92" s="40"/>
     </row>
     <row r="93" spans="1:8" ht="39" customHeight="1">
       <c r="A93" s="3"/>
@@ -2321,9 +3308,9 @@
       <c r="C93" s="4"/>
       <c r="D93" s="5"/>
       <c r="E93" s="23"/>
-      <c r="F93" s="34"/>
-      <c r="G93" s="35"/>
-      <c r="H93" s="36"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="39"/>
+      <c r="H93" s="40"/>
     </row>
     <row r="94" spans="1:8" ht="39" customHeight="1">
       <c r="A94" s="3"/>
@@ -2331,9 +3318,9 @@
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
       <c r="E94" s="23"/>
-      <c r="F94" s="34"/>
-      <c r="G94" s="35"/>
-      <c r="H94" s="36"/>
+      <c r="F94" s="38"/>
+      <c r="G94" s="39"/>
+      <c r="H94" s="40"/>
     </row>
     <row r="95" spans="1:8" ht="39" customHeight="1">
       <c r="A95" s="3"/>
@@ -2341,9 +3328,9 @@
       <c r="C95" s="4"/>
       <c r="D95" s="5"/>
       <c r="E95" s="23"/>
-      <c r="F95" s="34"/>
-      <c r="G95" s="35"/>
-      <c r="H95" s="36"/>
+      <c r="F95" s="38"/>
+      <c r="G95" s="39"/>
+      <c r="H95" s="40"/>
     </row>
     <row r="96" spans="1:8" ht="39" customHeight="1">
       <c r="A96" s="3"/>
@@ -2351,9 +3338,9 @@
       <c r="C96" s="4"/>
       <c r="D96" s="5"/>
       <c r="E96" s="23"/>
-      <c r="F96" s="34"/>
-      <c r="G96" s="35"/>
-      <c r="H96" s="36"/>
+      <c r="F96" s="38"/>
+      <c r="G96" s="39"/>
+      <c r="H96" s="40"/>
     </row>
     <row r="97" spans="1:8" ht="39" customHeight="1">
       <c r="A97" s="3"/>
@@ -2361,9 +3348,9 @@
       <c r="C97" s="4"/>
       <c r="D97" s="5"/>
       <c r="E97" s="23"/>
-      <c r="F97" s="34"/>
-      <c r="G97" s="35"/>
-      <c r="H97" s="36"/>
+      <c r="F97" s="38"/>
+      <c r="G97" s="39"/>
+      <c r="H97" s="40"/>
     </row>
     <row r="98" spans="1:8" ht="39" customHeight="1">
       <c r="A98" s="3"/>
@@ -2371,9 +3358,9 @@
       <c r="C98" s="4"/>
       <c r="D98" s="5"/>
       <c r="E98" s="23"/>
-      <c r="F98" s="34"/>
-      <c r="G98" s="35"/>
-      <c r="H98" s="36"/>
+      <c r="F98" s="38"/>
+      <c r="G98" s="39"/>
+      <c r="H98" s="40"/>
     </row>
     <row r="99" spans="1:8" ht="39" customHeight="1">
       <c r="A99" s="3"/>
@@ -2381,9 +3368,9 @@
       <c r="C99" s="4"/>
       <c r="D99" s="5"/>
       <c r="E99" s="23"/>
-      <c r="F99" s="34"/>
-      <c r="G99" s="35"/>
-      <c r="H99" s="36"/>
+      <c r="F99" s="38"/>
+      <c r="G99" s="39"/>
+      <c r="H99" s="40"/>
     </row>
     <row r="100" spans="1:8" ht="39" customHeight="1">
       <c r="A100" s="3"/>
@@ -2391,13 +3378,103 @@
       <c r="C100" s="4"/>
       <c r="D100" s="5"/>
       <c r="E100" s="23"/>
-      <c r="F100" s="34"/>
-      <c r="G100" s="35"/>
-      <c r="H100" s="36"/>
+      <c r="F100" s="38"/>
+      <c r="G100" s="39"/>
+      <c r="H100" s="40"/>
     </row>
     <row r="101" spans="1:8" ht="39" hidden="1" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="104">
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -2412,100 +3489,10 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -2518,13 +3505,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="21.875" style="17" customWidth="1"/>
     <col min="2" max="4" width="15" style="17" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="17" customWidth="1"/>
     <col min="6" max="16384" width="15" style="17" hidden="1"/>
@@ -2534,77 +3521,85 @@
       <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" ht="36" customHeight="1">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59"/>
-    </row>
-    <row r="3" spans="1:5" ht="136" customHeight="1">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+    </row>
+    <row r="3" spans="1:5" ht="135.94999999999999" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61"/>
-    </row>
-    <row r="4" spans="1:5" ht="46" customHeight="1">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="62"/>
+    </row>
+    <row r="4" spans="1:5" ht="45.95" customHeight="1">
       <c r="A4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="66"/>
-    </row>
-    <row r="5" spans="1:5" ht="46" customHeight="1">
+      <c r="B4" s="65">
+        <v>300</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="67"/>
+    </row>
+    <row r="5" spans="1:5" ht="45.95" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="61"/>
-    </row>
-    <row r="6" spans="1:5" ht="46" customHeight="1">
+      <c r="B5" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62"/>
+    </row>
+    <row r="6" spans="1:5" ht="45.95" customHeight="1">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="61"/>
-    </row>
-    <row r="7" spans="1:5" ht="46" customHeight="1">
+      <c r="B6" s="61">
+        <v>2</v>
+      </c>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62"/>
+    </row>
+    <row r="7" spans="1:5" ht="45.95" customHeight="1">
       <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
+      <c r="B7" s="65">
+        <v>6</v>
+      </c>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="1:5" ht="51" customHeight="1" thickBot="1">
       <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2619,7 +3614,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -2632,217 +3627,217 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="36" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="2" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2" hidden="1"/>
+    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
+    <col min="2" max="6" width="10.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1">
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="78">
+      <c r="B2" s="71">
         <v>41743</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="62"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
-    </row>
-    <row r="4" spans="1:7" ht="112" customHeight="1">
+      <c r="B3" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
+    </row>
+    <row r="4" spans="1:7" ht="111.95" customHeight="1">
       <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
+      <c r="B4" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
     </row>
     <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="63"/>
+      <c r="B5" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64"/>
     </row>
     <row r="6" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
     <row r="7" spans="1:7" ht="36" customHeight="1">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:7" ht="36" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="75"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="73"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
-    </row>
-    <row r="10" spans="1:7" ht="112" customHeight="1">
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+    </row>
+    <row r="10" spans="1:7" ht="111.95" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="61"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="77"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1"/>
     <row r="14" spans="1:7" ht="36" customHeight="1">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="70"/>
     </row>
     <row r="15" spans="1:7" ht="36" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="71"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="77"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
-    </row>
-    <row r="17" spans="1:7" ht="113" customHeight="1">
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62"/>
+    </row>
+    <row r="17" spans="1:7" ht="113.1" customHeight="1">
       <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
     </row>
     <row r="18" spans="1:7" ht="36" customHeight="1" thickBot="1">
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="73"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="79"/>
     </row>
     <row r="19" spans="1:7" ht="36" customHeight="1"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
@@ -2857,7 +3852,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>